<commit_message>
🔄️ Update Seleksi, Tambah Update Status Wawancara dan logika rekrut Pelamar
</commit_message>
<xml_diff>
--- a/data_rekrutmen.xlsx
+++ b/data_rekrutmen.xlsx
@@ -3,16 +3,17 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Lowongan" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Pelamar" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Wawancara" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Seleksi" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -48,14 +49,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -137,10 +132,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -178,71 +173,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -270,7 +265,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -293,11 +288,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -306,13 +301,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -322,7 +317,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -331,7 +326,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -340,7 +335,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -348,10 +343,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -427,7 +422,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -445,97 +440,94 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <cols>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="1" max="1"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="2" max="2"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="3" max="3"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="4" max="4"/>
+    <col width="13.54296875" bestFit="1" customWidth="1" min="1" max="4"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75" customHeight="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>Kode</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>Posisi</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>Deskripsi</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
     </row>
     <row r="2" ht="18.75" customHeight="1">
-      <c r="A2" s="2" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t>L001</t>
         </is>
       </c>
-      <c r="B2" s="2" t="inlineStr">
+      <c r="B2" t="inlineStr">
         <is>
           <t>IT Consultan</t>
         </is>
       </c>
-      <c r="C2" s="2" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>Bekerja menjadi IT Consultan</t>
         </is>
       </c>
-      <c r="D2" s="2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>Dibuka</t>
         </is>
       </c>
     </row>
     <row r="3" ht="18.75" customHeight="1">
-      <c r="A3" s="2" t="inlineStr">
+      <c r="A3" t="inlineStr">
         <is>
           <t>L002</t>
         </is>
       </c>
-      <c r="B3" s="2" t="inlineStr">
+      <c r="B3" t="inlineStr">
         <is>
           <t>IT Network</t>
         </is>
       </c>
-      <c r="C3" s="2" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>Bekerja menjadi IT Network</t>
         </is>
       </c>
-      <c r="D3" s="2" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>Dibuka</t>
         </is>
       </c>
     </row>
     <row r="4" ht="18.75" customHeight="1">
-      <c r="A4" s="2" t="inlineStr">
+      <c r="A4" t="inlineStr">
         <is>
           <t>L003</t>
         </is>
       </c>
-      <c r="B4" s="2" t="inlineStr">
+      <c r="B4" t="inlineStr">
         <is>
           <t>Proggrammer</t>
         </is>
       </c>
-      <c r="C4" s="2" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>Koding Sampe Gila</t>
         </is>
       </c>
-      <c r="D4" s="2" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>Dibuka</t>
         </is>
@@ -554,122 +546,118 @@
   </sheetPr>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <cols>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="1" max="1"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="2" max="2"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="3" max="3"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="4" max="4"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="5" max="5"/>
+    <col width="13.54296875" bestFit="1" customWidth="1" min="1" max="5"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75" customHeight="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>Kode Pelamar</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>Nama</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>Kontak</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>Posisi Dilamar</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>Status Wawancara</t>
         </is>
       </c>
     </row>
     <row r="2" ht="18.75" customHeight="1">
-      <c r="A2" s="2" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t>P001</t>
         </is>
       </c>
-      <c r="B2" s="2" t="inlineStr">
+      <c r="B2" t="inlineStr">
         <is>
           <t>Agus</t>
         </is>
       </c>
-      <c r="C2" s="2" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>1231</t>
         </is>
       </c>
-      <c r="D2" s="2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>Proggrammer</t>
         </is>
       </c>
-      <c r="E2" s="2" t="inlineStr">
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Selesai</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="18.75" customHeight="1">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>P002</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Ahmad</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2311</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Proggrammer</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
         <is>
           <t>Proses</t>
         </is>
       </c>
     </row>
-    <row r="3" ht="18.75" customHeight="1">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>P002</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="inlineStr">
-        <is>
-          <t>Ahmad</t>
-        </is>
-      </c>
-      <c r="C3" s="2" t="inlineStr">
-        <is>
-          <t>2311</t>
-        </is>
-      </c>
-      <c r="D3" s="2" t="inlineStr">
+    <row r="4" ht="18.75" customHeight="1">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>P003</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Jidan</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2093</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
         <is>
           <t>Proggrammer</t>
         </is>
       </c>
-      <c r="E3" s="2" t="inlineStr">
-        <is>
-          <t>Proses</t>
-        </is>
-      </c>
-    </row>
-    <row r="4" ht="18.75" customHeight="1">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>P003</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="inlineStr">
-        <is>
-          <t>Jidan</t>
-        </is>
-      </c>
-      <c r="C4" s="2" t="inlineStr">
-        <is>
-          <t>2093</t>
-        </is>
-      </c>
-      <c r="D4" s="2" t="inlineStr">
-        <is>
-          <t>Proggrammer</t>
-        </is>
-      </c>
-      <c r="E4" s="2" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>Belum</t>
         </is>
@@ -688,117 +676,175 @@
   </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <cols>
+    <col width="13.54296875" bestFit="1" customWidth="1" min="1" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="18.75" customHeight="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Kode Lowongan</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Kode Pelamar</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Nama Pelamar</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Posisi</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Jadwal Tanggal</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Jadwal Jam</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="18.75" customHeight="1">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>L003</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>P001</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Agus</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Proggrammer</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2024-03-21</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>13.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>L003</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>P002</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Ahmad</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Proggrammer</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2024-04-30</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>08.00</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="1" max="1"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="2" max="2"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="3" max="3"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="4" max="4"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="5" max="5"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="6" max="6"/>
-  </cols>
   <sheetData>
-    <row r="1" ht="18.75" customHeight="1">
-      <c r="A1" s="2" t="inlineStr">
-        <is>
-          <t>Kode Lowongan</t>
-        </is>
-      </c>
-      <c r="B1" s="2" t="inlineStr">
+    <row r="1">
+      <c r="A1" t="inlineStr">
         <is>
           <t>Kode Pelamar</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
-        <is>
-          <t>Nama Pelamar</t>
-        </is>
-      </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Nama</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
         <is>
           <t>Posisi</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
-        <is>
-          <t>Jadwal Tanggal</t>
-        </is>
-      </c>
-      <c r="F1" s="2" t="inlineStr">
-        <is>
-          <t>Jadwal Jam</t>
-        </is>
-      </c>
-    </row>
-    <row r="2" ht="18.75" customHeight="1">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>L003</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="inlineStr">
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Status Seleksi</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
         <is>
           <t>P001</t>
         </is>
       </c>
-      <c r="C2" s="2" t="inlineStr">
+      <c r="B2" t="inlineStr">
         <is>
           <t>Agus</t>
         </is>
       </c>
-      <c r="D2" s="2" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>Proggrammer</t>
         </is>
       </c>
-      <c r="E2" s="2" t="inlineStr">
-        <is>
-          <t>2024-03-21</t>
-        </is>
-      </c>
-      <c r="F2" s="2" t="inlineStr">
-        <is>
-          <t>13.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>L003</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>P002</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Ahmad</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Proggrammer</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>2024-04-30</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>08.00</t>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Diterima</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
🔄️ Update edit & delete function Lowongan
</commit_message>
<xml_diff>
--- a/data_rekrutmen.xlsx
+++ b/data_rekrutmen.xlsx
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -528,6 +528,28 @@
         </is>
       </c>
       <c r="D4" t="inlineStr">
+        <is>
+          <t>Dibuka</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>L004</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Operator Mesin</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Whuthedel</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
         <is>
           <t>Dibuka</t>
         </is>

</xml_diff>

<commit_message>
🔄️ Update tampil, edit & delete membuat tampilan lebih friendly user
</commit_message>
<xml_diff>
--- a/data_rekrutmen.xlsx
+++ b/data_rekrutmen.xlsx
@@ -11,6 +11,7 @@
     <sheet name="Pelamar" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Wawancara" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="Seleksi" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Penawaran" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -869,4 +870,47 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Kode Pekerjaan</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Benefit</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>L001</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Asuransi Kecelakaan Kerja</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
🔄️Update Tambah, Edit dan Delete Wawancara supaya lebih friendly
</commit_message>
<xml_diff>
--- a/data_rekrutmen.xlsx
+++ b/data_rekrutmen.xlsx
@@ -3,15 +3,14 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Lowongan" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Pelamar" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Wawancara" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Seleksi" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Penawaran" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Penawaran" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Wawancara" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -534,7 +533,7 @@
         </is>
       </c>
     </row>
-    <row r="5">
+    <row r="5" ht="18.75" customHeight="1">
       <c r="A5" t="inlineStr">
         <is>
           <t>L004</t>
@@ -569,8 +568,8 @@
   </sheetPr>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
@@ -628,7 +627,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Selesai</t>
+          <t>Belum</t>
         </is>
       </c>
     </row>
@@ -655,7 +654,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Proses</t>
+          <t>Belum</t>
         </is>
       </c>
     </row>
@@ -682,7 +681,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Belum</t>
+          <t>Proses</t>
         </is>
       </c>
     </row>
@@ -697,110 +696,50 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <cols>
-    <col width="13.54296875" bestFit="1" customWidth="1" min="1" max="6"/>
+    <col width="13.54296875" bestFit="1" customWidth="1" min="1" max="2"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75" customHeight="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Kode Lowongan</t>
+          <t>Kode Pekerjaan</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Kode Pelamar</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Nama Pelamar</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Posisi</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Jadwal Tanggal</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Jadwal Jam</t>
+          <t>Benefit</t>
         </is>
       </c>
     </row>
     <row r="2" ht="18.75" customHeight="1">
       <c r="A2" t="inlineStr">
         <is>
-          <t>L003</t>
+          <t>L001</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>P001</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Agus</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Proggrammer</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>2024-03-21</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>13.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
+          <t>Asuransi Kesehatan</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="18.75" customHeight="1">
       <c r="A3" t="inlineStr">
         <is>
-          <t>L003</t>
+          <t>L001</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>P002</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Ahmad</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Proggrammer</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>2024-04-30</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>08.00</t>
+          <t>Uang Transport</t>
         </is>
       </c>
     </row>
@@ -815,7 +754,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -826,87 +765,64 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>Kode Lowongan</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
           <t>Kode Pelamar</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Nama</t>
-        </is>
-      </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>Nama Pelamar</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>Posisi</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Status Seleksi</t>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Jadwal Tanggal</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Jadwal Jam</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>P001</t>
+          <t>L003</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Agus</t>
+          <t>P003</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>Jidan</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t>Proggrammer</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Diterima</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Kode Pekerjaan</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Benefit</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>L001</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Asuransi Kecelakaan Kerja</t>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2024-07-03</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>18.00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🔄️ Update function Update Status Wawancara hilangkan if "Seleksi"
</commit_message>
<xml_diff>
--- a/data_rekrutmen.xlsx
+++ b/data_rekrutmen.xlsx
@@ -11,6 +11,7 @@
     <sheet name="Pelamar" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Penawaran" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="Wawancara" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Seleksi" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -627,7 +628,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Belum</t>
+          <t>Selesai</t>
         </is>
       </c>
     </row>
@@ -754,7 +755,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -826,6 +827,101 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>L003</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>P001</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Haji Ahda</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Proggrammer</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2024-01-20</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>16.00</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Kode Pelamar</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Nama</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Posisi</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Status Seleksi</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>P001</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Haji Ahda</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Proggrammer</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Diterima</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>